<commit_message>
actualización base de datos excel
</commit_message>
<xml_diff>
--- a/instrumentos.xlsx
+++ b/instrumentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUAN RAMIREZ\Desktop\pruebas-git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A244502F-E4FD-4CA1-9605-57E244E2701A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80BB68E-B043-4467-8C5C-5BB0607DE11E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="0" windowWidth="20295" windowHeight="10920" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PM TRANS" sheetId="1" r:id="rId1"/>
@@ -6305,31 +6305,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="102">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial Narrow"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -6968,6 +6943,31 @@
         <name val="Arial Narrow"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -8342,58 +8342,58 @@
     <tableColumn id="29" xr3:uid="{00000000-0010-0000-0300-00001D000000}" name="MARCA" dataDxfId="40"/>
     <tableColumn id="30" xr3:uid="{00000000-0010-0000-0300-00001E000000}" name="MODELO" dataDxfId="39"/>
     <tableColumn id="31" xr3:uid="{00000000-0010-0000-0300-00001F000000}" name="SERIE" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{8B8112D1-F8C4-412B-9E4B-A19D40E27521}" name="CRITICIDAD" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="FREC." dataDxfId="37"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0300-000020000000}" name="ESTADO" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="PMA" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{8B8112D1-F8C4-412B-9E4B-A19D40E27521}" name="CRITICIDAD" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="FREC." dataDxfId="36"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0300-000020000000}" name="ESTADO" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="PMA" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="DB_ENVASADO" displayName="DB_ENVASADO" ref="A1:O82" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="DB_ENVASADO" displayName="DB_ENVASADO" ref="A1:O82" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:O82" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="ITEM" dataDxfId="32"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0500-00001A000000}" name="TAG" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="TIPO EQUIPO" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="SERVICIO" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="DEPARTAMENTO" dataDxfId="28"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0500-00001C000000}" name="ETAPA" dataDxfId="27"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0500-00001D000000}" name="DENOMINACION" dataDxfId="26"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0500-00001B000000}" name="EQUIPO" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="MARCA" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="MODELO" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="SERIE" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="CRITICIDAD" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="TIPO 1" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="ESTADO" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="PMA" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="ITEM" dataDxfId="31"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0500-00001A000000}" name="TAG" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="TIPO EQUIPO" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="SERVICIO" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="DEPARTAMENTO" dataDxfId="27"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0500-00001C000000}" name="ETAPA" dataDxfId="26"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0500-00001D000000}" name="DENOMINACION" dataDxfId="25"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0500-00001B000000}" name="EQUIPO" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="MARCA" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="MODELO" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="SERIE" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="CRITICIDAD" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="TIPO 1" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="ESTADO" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="PMA" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="DB_DVM" displayName="DB_DVM" ref="A1:O30" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="DB_DVM" displayName="DB_DVM" ref="A1:O30" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:O30" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="ITEM" dataDxfId="15"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0600-00001A000000}" name="TAG" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="TIPO EQUIPO" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="SERVICIO" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="DEPARTAMENTO" dataDxfId="11"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0600-00001C000000}" name="ETAPA" dataDxfId="10"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0600-00001D000000}" name="DENOMINACION" dataDxfId="9"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0600-00001B000000}" name="EQUIPO" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="MARCA" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="MODELO" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="SERIE" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="CRITICIDAD" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="ESTADO" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="PMA" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="TIPO 1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="ITEM" dataDxfId="14"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0600-00001A000000}" name="TAG" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="TIPO EQUIPO" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="SERVICIO" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="DEPARTAMENTO" dataDxfId="10"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0600-00001C000000}" name="ETAPA" dataDxfId="9"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0600-00001D000000}" name="DENOMINACION" dataDxfId="8"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0600-00001B000000}" name="EQUIPO" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="MARCA" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="MODELO" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="SERIE" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="CRITICIDAD" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="ESTADO" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="PMA" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="TIPO 1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8678,7 +8678,7 @@
   </sheetPr>
   <dimension ref="A1:Q839"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
@@ -44109,7 +44109,7 @@
   </sheetPr>
   <dimension ref="A1:AC198"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>

</xml_diff>